<commit_message>
excel sheet is now expandable
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Names</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>B2</t>
+  </si>
+  <si>
+    <t>Aarush</t>
+  </si>
+  <si>
+    <t>C1</t>
   </si>
 </sst>
 </file>
@@ -53,7 +59,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +70,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -95,15 +107,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -414,15 +429,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -436,7 +451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -445,7 +460,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="1"/>
       <c r="B3" s="3">
         <v>90</v>
@@ -459,7 +474,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -468,7 +483,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3">
         <v>90</v>
@@ -482,7 +497,7 @@
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -491,7 +506,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="1"/>
       <c r="B9" s="3">
         <v>85</v>
@@ -505,7 +520,7 @@
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -516,11 +531,34 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1"/>
-      <c r="B12" s="3">
+      <c r="B12" s="4">
         <v>79</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4">
+        <v>150</v>
+      </c>
+      <c r="C14" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3">
+        <v>56</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>